<commit_message>
hang san xuat & loai hang
</commit_message>
<xml_diff>
--- a/QLCC/QLCC/wwwroot/filemau/filemau_dichvucoban.xlsx
+++ b/QLCC/QLCC/wwwroot/filemau/filemau_dichvucoban.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>A2</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>denNgay</t>
+  </si>
+  <si>
+    <t>03-08-2018T00:00:00</t>
+  </si>
+  <si>
+    <t>03-11-2018T00:00:00</t>
   </si>
 </sst>
 </file>
@@ -60,7 +66,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,###"/>
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -427,14 +433,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -473,8 +479,8 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>43315</v>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>100000</v>
@@ -486,8 +492,8 @@
         <f>C2*D2</f>
         <v>100000</v>
       </c>
-      <c r="F2" s="4">
-        <v>43315</v>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
@@ -495,11 +501,11 @@
       <c r="H2" s="2">
         <v>100000</v>
       </c>
-      <c r="I2" s="4">
-        <v>43315</v>
-      </c>
-      <c r="J2" s="4">
-        <v>43315</v>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>